<commit_message>
new tab & .xlsx file fix
</commit_message>
<xml_diff>
--- a/BD_version_1.xlsx
+++ b/BD_version_1.xlsx
@@ -5,18 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sonan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Pycharm projects\Polyakov\3BR-base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BFB9EC-3C4E-4EED-A292-5539E1E9EF03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB2448B1-AC6A-4CB3-8447-080F5D5C7AC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22890" yWindow="4740" windowWidth="11565" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -445,7 +444,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,10 +471,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -495,10 +494,10 @@
         <v>17</v>
       </c>
       <c r="F2">
+        <v>40</v>
+      </c>
+      <c r="G2">
         <v>2600</v>
-      </c>
-      <c r="G2">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -518,10 +517,10 @@
         <v>17</v>
       </c>
       <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3">
         <v>2500</v>
-      </c>
-      <c r="G3">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -541,10 +540,10 @@
         <v>19</v>
       </c>
       <c r="F4">
+        <v>40</v>
+      </c>
+      <c r="G4">
         <v>2100</v>
-      </c>
-      <c r="G4">
-        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -564,10 +563,10 @@
         <v>18</v>
       </c>
       <c r="F5">
+        <v>40</v>
+      </c>
+      <c r="G5">
         <v>2300</v>
-      </c>
-      <c r="G5">
-        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -587,10 +586,10 @@
         <v>17</v>
       </c>
       <c r="F6">
+        <v>40</v>
+      </c>
+      <c r="G6">
         <v>2550</v>
-      </c>
-      <c r="G6">
-        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -610,10 +609,10 @@
         <v>18</v>
       </c>
       <c r="F7">
+        <v>40</v>
+      </c>
+      <c r="G7">
         <v>2150</v>
-      </c>
-      <c r="G7">
-        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -633,10 +632,10 @@
         <v>19</v>
       </c>
       <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8">
         <v>2200</v>
-      </c>
-      <c r="G8">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -656,10 +655,10 @@
         <v>18</v>
       </c>
       <c r="F9">
+        <v>30</v>
+      </c>
+      <c r="G9">
         <v>2400</v>
-      </c>
-      <c r="G9">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -679,10 +678,10 @@
         <v>17</v>
       </c>
       <c r="F10">
+        <v>40</v>
+      </c>
+      <c r="G10">
         <v>2350</v>
-      </c>
-      <c r="G10">
-        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -702,10 +701,10 @@
         <v>19</v>
       </c>
       <c r="F11">
+        <v>30</v>
+      </c>
+      <c r="G11">
         <v>1950</v>
-      </c>
-      <c r="G11">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>